<commit_message>
Refactored to have common skeletal code for manifests, and support multiple manifests in a single Excel posting
</commit_message>
<xml_diff>
--- a/apodeixi/controllers/kernel/bdd/tests_unit/input_data/feature_injection_INPUT.xlsx
+++ b/apodeixi/controllers/kernel/bdd/tests_unit/input_data/feature_injection_INPUT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\apodeixi\controllers\kernel\bdd\test_unit\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\Code\chateauclaudia-labs\apodeixi\project\apodeixi\controllers\kernel\bdd\tests_unit\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3879AA19-1F70-4D0D-9559-FFFCC0CEAE48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68756F34-C136-48E9-A976-F2A566F22BA4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" activeTab="1" xr2:uid="{4B727691-5255-46C4-A89F-234F9FDCAFEC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="122">
   <si>
     <t>Journeys</t>
   </si>
@@ -313,9 +313,6 @@
     <t>alejandro@chateauclaudia-labs.com</t>
   </si>
   <si>
-    <t>dataRange</t>
-  </si>
-  <si>
     <t>"what'</t>
   </si>
   <si>
@@ -370,9 +367,6 @@
     <t>excelAPI</t>
   </si>
   <si>
-    <t>capability-hierarchy.kernel.a6i.xlsx/v1a</t>
-  </si>
-  <si>
     <t>Posting Label</t>
   </si>
   <si>
@@ -395,6 +389,18 @@
   </si>
   <si>
     <t>scaffoldingPurpose</t>
+  </si>
+  <si>
+    <t>bdd.kernel.a6i.xlsx/v1a</t>
+  </si>
+  <si>
+    <t>capability-hierarchy</t>
+  </si>
+  <si>
+    <t>data.kind</t>
+  </si>
+  <si>
+    <t>data.range</t>
   </si>
 </sst>
 </file>
@@ -1096,7 +1102,7 @@
   <dimension ref="B1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C19" sqref="C18:C19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1116,7 +1122,7 @@
   <sheetData>
     <row r="1" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B1" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M1" s="16" t="s">
         <v>78</v>
@@ -1128,10 +1134,10 @@
     </row>
     <row r="2" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B2" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>75</v>
@@ -1145,12 +1151,12 @@
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
     </row>
-    <row r="3" spans="2:17" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>119</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>118</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>63</v>
@@ -1169,7 +1175,7 @@
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="8" t="s">
         <v>117</v>
       </c>
@@ -1177,55 +1183,55 @@
         <v>116</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.45">
       <c r="B5" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>115</v>
-      </c>
       <c r="E5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>74</v>
@@ -1234,7 +1240,7 @@
         <v>76</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>67</v>
@@ -1243,18 +1249,18 @@
         <v>79</v>
       </c>
       <c r="P5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="6" spans="2:17" s="5" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B6" s="8" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>81</v>
@@ -1296,10 +1302,10 @@
     </row>
     <row r="7" spans="2:17" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B7" s="8" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -1319,10 +1325,10 @@
     </row>
     <row r="8" spans="2:17" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B8" s="8" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>62</v>
@@ -1362,8 +1368,12 @@
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.45">
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
+      <c r="B9" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="M9" s="2" t="s">
         <v>68</v>
       </c>

</xml_diff>